<commit_message>
social media activity by attribute
</commit_message>
<xml_diff>
--- a/data/analysis/social_media_analytics/museums_on_tw_temporal-all_mus-D.xlsx
+++ b/data/analysis/social_media_analytics/museums_on_tw_temporal-all_mus-D.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="4">
   <si>
     <t>ts</t>
   </si>
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1006"/>
+  <dimension ref="A1:C1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -11448,17 +11448,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="1006" spans="1:3">
-      <c r="A1006" s="2">
-        <v>44470</v>
-      </c>
-      <c r="B1006">
-        <v>1</v>
-      </c>
-      <c r="C1006" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>